<commit_message>
remove enter window, adding to info directly
</commit_message>
<xml_diff>
--- a/amazon_scraping_items/itemList.xlsx
+++ b/amazon_scraping_items/itemList.xlsx
@@ -51,67 +51,67 @@
     <t>Holy Stone GPS FPV RC Drone HS100 with Camera Live Video and GPS Return Home Quadcopter with Adjustable Wide-Angle 720P HD WIFI Camera- Follow Me, Altitude Hold, Intelligent Battery Long Control Range</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Adjustable-Intelligent/dp/B074YYVXQH/ref=sr_1_4?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-4&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>4.6 out of 5 stars</t>
   </si>
   <si>
     <t>Drone With Camera Live Video, EACHINE E58 WIFI FPV Quadcopter With 120° Wide-angle 720P HD Camera Foldable Drone RTF - Altitude Hold, One Key Take Off/Landing, 3D Flip, APP Control, Gravity Sensor</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Camera-EACHINE-Quadcopter-Wide-angle-Foldable/dp/B0776QJNS3/ref=sr_1_5?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-5&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>4.2 out of 5 stars</t>
   </si>
   <si>
     <t>Holy Stone HS170 Predator Mini RC Helicopter Drone 2.4Ghz 6-Axis Gyro 4 Channels Quadcopter Good Choice for Drone Training</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Holy-Stone-Predator-Helicopter-Quadcopter/dp/B0157IHJMQ/ref=sr_1_6?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-6&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>4.4 out of 5 stars</t>
   </si>
   <si>
     <t>Holy Stone HS160 Shadow FPV RC Drone with 720P HD Wi-Fi Camera Live Video Feed 2.4GHz 6-Axis Gyro Quadcopter for Kids &amp; Beginners - Altitude Hold, One Key Start, Foldable Arms,Bonus Battery</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Holy-Stone-Shadow-Quadcopter-Beginners/dp/B074S2HK59/ref=sr_1_7?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-7&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>4.3 out of 5 stars</t>
   </si>
   <si>
     <t>DROCON Drone For Beginners X708W Wi-Fi FPV Training Quadcopter With HD Camera Equipped With Headless Mode One Key Return Easy Operation</t>
   </si>
   <si>
-    <t>https://www.amazon.com/DROCON-Beginners-Training-Quadcopter-Operation/dp/B073HYDPT3/ref=sr_1_8?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-8&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>3.9 out of 5 stars</t>
   </si>
   <si>
     <t>Cheerwing Syma X5SW-V3 FPV Explorers2 2.4Ghz 4CH 6-Axis Gyro RC Headless Quadcopter Drone UFO with HD Wifi Camera (White)</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Cheerwing-X5SW-V3-Explorers2-Headless-Quadcopter/dp/B011JV9HA2/ref=sr_1_10?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-10&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>3.7 out of 5 stars</t>
   </si>
   <si>
     <t>LBLA FPV Drone with Wifi Camera Live Video Headless Mode 2.4GHz 4 CH 6 Axis Gyro RTF RC Quadcopter, Compatible with 3D VR Headset</t>
   </si>
   <si>
-    <t>https://www.amazon.com/LBLA-Headless-Quadcopter-Compatible-Headset/dp/B077BZQ8JZ/ref=sr_1_12?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-12&amp;keywords=drone</t>
-  </si>
-  <si>
     <t>Holy Stone F181C RC Quadcopter Drone with HD Camera RTF 4 Channel 2.4GHz 6-Gyro with Altitude Hold Function,Headless Mode and One Key Return Home, Color Black</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Altitude-Function/dp/B00SAUAP5C/ref=sr_1_16?s=toys-and-games&amp;ie=UTF8&amp;qid=1527885793&amp;sr=1-16&amp;keywords=drone</t>
+    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Adjustable-Intelligent/dp/B074YYVXQH/ref=sr_1_4?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-4&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Camera-EACHINE-Quadcopter-Wide-angle-Foldable/dp/B0776QJNS3/ref=sr_1_5?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-5&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Predator-Helicopter-Quadcopter/dp/B0157IHJMQ/ref=sr_1_6?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-6&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Shadow-Quadcopter-Beginners/dp/B074S2HK59/ref=sr_1_7?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-7&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DROCON-Beginners-Training-Quadcopter-Operation/dp/B073HYDPT3/ref=sr_1_8?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-8&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Cheerwing-X5SW-V3-Explorers2-Headless-Quadcopter/dp/B011JV9HA2/ref=sr_1_10?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-10&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LBLA-Headless-Quadcopter-Compatible-Headset/dp/B077BZQ8JZ/ref=sr_1_12?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-12&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Altitude-Function/dp/B00SAUAP5C/ref=sr_1_16?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-16&amp;keywords=drone</t>
   </si>
 </sst>
 </file>
@@ -458,10 +458,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2">
         <v>930</v>
@@ -472,13 +472,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>226</v>
@@ -489,13 +489,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>4463</v>
@@ -506,13 +506,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>1011</v>
@@ -523,13 +523,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>737</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>4629</v>
@@ -551,13 +551,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
         <v>1511</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>1174</v>
@@ -579,13 +579,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>54</v>
@@ -596,13 +596,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
         <v>3001</v>
@@ -646,10 +646,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2">
         <v>930</v>
@@ -660,13 +660,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>226</v>
@@ -677,13 +677,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>4463</v>
@@ -694,13 +694,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>1011</v>
@@ -711,13 +711,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>737</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>4629</v>
@@ -739,13 +739,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
         <v>1511</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>1174</v>
@@ -767,13 +767,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>54</v>
@@ -784,13 +784,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
         <v>3001</v>

</xml_diff>

<commit_message>
auto-adding close terminal action
</commit_message>
<xml_diff>
--- a/amazon_scraping_items/itemList.xlsx
+++ b/amazon_scraping_items/itemList.xlsx
@@ -90,28 +90,28 @@
     <t>Holy Stone F181C RC Quadcopter Drone with HD Camera RTF 4 Channel 2.4GHz 6-Gyro with Altitude Hold Function,Headless Mode and One Key Return Home, Color Black</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Adjustable-Intelligent/dp/B074YYVXQH/ref=sr_1_4?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-4&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Camera-EACHINE-Quadcopter-Wide-angle-Foldable/dp/B0776QJNS3/ref=sr_1_5?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-5&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Holy-Stone-Predator-Helicopter-Quadcopter/dp/B0157IHJMQ/ref=sr_1_6?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-6&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Holy-Stone-Shadow-Quadcopter-Beginners/dp/B074S2HK59/ref=sr_1_7?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-7&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/DROCON-Beginners-Training-Quadcopter-Operation/dp/B073HYDPT3/ref=sr_1_8?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-8&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Cheerwing-X5SW-V3-Explorers2-Headless-Quadcopter/dp/B011JV9HA2/ref=sr_1_10?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-10&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/LBLA-Headless-Quadcopter-Compatible-Headset/dp/B077BZQ8JZ/ref=sr_1_12?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-12&amp;keywords=drone</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Altitude-Function/dp/B00SAUAP5C/ref=sr_1_16?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886567&amp;sr=1-16&amp;keywords=drone</t>
+    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Adjustable-Intelligent/dp/B074YYVXQH/ref=sr_1_4?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-4&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Camera-EACHINE-Quadcopter-Wide-angle-Foldable/dp/B0776QJNS3/ref=sr_1_5?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-5&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Predator-Helicopter-Quadcopter/dp/B0157IHJMQ/ref=sr_1_6?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-6&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Shadow-Quadcopter-Beginners/dp/B074S2HK59/ref=sr_1_7?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-7&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DROCON-Beginners-Training-Quadcopter-Operation/dp/B073HYDPT3/ref=sr_1_8?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-8&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Cheerwing-X5SW-V3-Explorers2-Headless-Quadcopter/dp/B011JV9HA2/ref=sr_1_10?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-10&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LBLA-Headless-Quadcopter-Compatible-Headset/dp/B077BZQ8JZ/ref=sr_1_12?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-12&amp;keywords=drone</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Holy-Stone-Quadcopter-Altitude-Function/dp/B00SAUAP5C/ref=sr_1_16?s=toys-and-games&amp;ie=UTF8&amp;qid=1527886721&amp;sr=1-16&amp;keywords=drone</t>
   </si>
 </sst>
 </file>

</xml_diff>